<commit_message>
Add plots for Scan, Sort with OpenCL
</commit_message>
<xml_diff>
--- a/reduce/plots/Float_Data.xlsx
+++ b/reduce/plots/Float_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="11328" windowHeight="3024" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="11328" windowHeight="3024" tabRatio="642" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reduce" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
   <si>
     <t>Thrust</t>
   </si>
@@ -174,15 +174,6 @@
     <t>OpenCL</t>
   </si>
   <si>
-    <t>Gflops</t>
-  </si>
-  <si>
-    <t>Copy time</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -190,12 +181,6 @@
   </si>
   <si>
     <t>No detect</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>here</t>
   </si>
   <si>
     <t>1_K20Xm</t>
@@ -238,6 +223,9 @@
   </si>
   <si>
     <t>Tesla_K40c_Thrust</t>
+  </si>
+  <si>
+    <t>FLOPS</t>
   </si>
 </sst>
 </file>
@@ -888,11 +876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="8418048"/>
-        <c:axId val="8419968"/>
+        <c:axId val="78730368"/>
+        <c:axId val="78732288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8418048"/>
+        <c:axId val="78730368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -928,13 +916,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8419968"/>
+        <c:crossAx val="78732288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8419968"/>
+        <c:axId val="78732288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8418048"/>
+        <c:crossAx val="78730368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1405,11 +1393,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="8504064"/>
-        <c:axId val="8505984"/>
+        <c:axId val="79905920"/>
+        <c:axId val="79907840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8504064"/>
+        <c:axId val="79905920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1438,19 +1426,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8505984"/>
+        <c:crossAx val="79907840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8505984"/>
+        <c:axId val="79907840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -1475,13 +1464,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8504064"/>
+        <c:crossAx val="79905920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1489,6 +1479,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2051,11 +2042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="8545792"/>
-        <c:axId val="8547712"/>
+        <c:axId val="78825344"/>
+        <c:axId val="78827520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8545792"/>
+        <c:axId val="78825344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2084,19 +2075,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8547712"/>
+        <c:crossAx val="78827520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8547712"/>
+        <c:axId val="78827520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2119,13 +2111,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8545792"/>
+        <c:crossAx val="78825344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -2133,6 +2126,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2825,11 +2819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="33475584"/>
-        <c:axId val="33481856"/>
+        <c:axId val="79986048"/>
+        <c:axId val="79992320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33475584"/>
+        <c:axId val="79986048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2858,19 +2852,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33481856"/>
+        <c:crossAx val="79992320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33481856"/>
+        <c:axId val="79992320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2893,13 +2888,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33475584"/>
+        <c:crossAx val="79986048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8"/>
@@ -2907,6 +2903,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3469,11 +3466,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="33542144"/>
-        <c:axId val="33544064"/>
+        <c:axId val="80397824"/>
+        <c:axId val="80399744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33542144"/>
+        <c:axId val="80397824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3502,19 +3499,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33544064"/>
+        <c:crossAx val="80399744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33544064"/>
+        <c:axId val="80399744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -3539,13 +3537,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33542144"/>
+        <c:crossAx val="80397824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -3553,6 +3552,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4765,11 +4765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="33657600"/>
-        <c:axId val="33659520"/>
+        <c:axId val="80521856"/>
+        <c:axId val="80614144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33657600"/>
+        <c:axId val="80521856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -4793,19 +4793,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33659520"/>
+        <c:crossAx val="80614144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33659520"/>
+        <c:axId val="80614144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -4835,13 +4836,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33657600"/>
+        <c:crossAx val="80521856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -4849,6 +4851,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5411,11 +5414,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="33732096"/>
-        <c:axId val="33734016"/>
+        <c:axId val="80948608"/>
+        <c:axId val="80958976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33732096"/>
+        <c:axId val="80948608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -5451,13 +5454,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33734016"/>
+        <c:crossAx val="80958976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33734016"/>
+        <c:axId val="80958976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -5489,7 +5492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33732096"/>
+        <c:crossAx val="80948608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -6302,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6316,20 +6319,20 @@
     <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F1" s="9"/>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -6342,17 +6345,8 @@
       <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -6360,19 +6354,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -6380,19 +6365,16 @@
         <v>19</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6400,19 +6382,16 @@
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -6420,19 +6399,16 @@
         <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -6440,19 +6416,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -6460,16 +6430,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -6477,16 +6444,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -6494,19 +6458,24 @@
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>3</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6518,7 +6487,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6537,7 +6506,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -6549,21 +6518,6 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6583,21 +6537,10 @@
       <c r="E2">
         <v>29.167999999999999</v>
       </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2" s="8">
-        <v>7.8701499999999995E-6</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1.0212300000000001E-2</v>
-      </c>
-      <c r="K2" s="8">
-        <v>1.01216E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1.03021E-2</v>
-      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -6615,21 +6558,10 @@
       <c r="E3">
         <v>28.975300000000001</v>
       </c>
-      <c r="H3">
-        <v>11</v>
-      </c>
-      <c r="I3" s="8">
-        <v>8.7738900000000001E-6</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1.10026E-2</v>
-      </c>
-      <c r="K3" s="8">
-        <v>1.0852499999999999E-2</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1.10659E-2</v>
-      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -6647,21 +6579,10 @@
       <c r="E4">
         <v>27.391400000000001</v>
       </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4" s="8">
-        <v>9.6574500000000002E-6</v>
-      </c>
-      <c r="J4" s="8">
-        <v>1.1683799999999999E-2</v>
-      </c>
-      <c r="K4" s="8">
-        <v>1.15146E-2</v>
-      </c>
-      <c r="L4" s="8">
-        <v>1.16834E-2</v>
-      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -6679,21 +6600,10 @@
       <c r="E5">
         <v>28.2272</v>
       </c>
-      <c r="H5">
-        <v>13</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1.1994800000000001E-5</v>
-      </c>
-      <c r="J5" s="8">
-        <v>1.4233300000000001E-2</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1.40524E-2</v>
-      </c>
-      <c r="L5" s="8">
-        <v>1.43328E-2</v>
-      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -6711,21 +6621,10 @@
       <c r="E6">
         <v>28.500800000000002</v>
       </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6" s="8">
-        <v>1.49088E-5</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1.6916299999999999E-2</v>
-      </c>
-      <c r="K6" s="8">
-        <v>1.6641599999999999E-2</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1.6879499999999999E-2</v>
-      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -6743,21 +6642,10 @@
       <c r="E7">
         <v>29.299399999999999</v>
       </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1.62122E-5</v>
-      </c>
-      <c r="J7" s="8">
-        <v>1.91827E-2</v>
-      </c>
-      <c r="K7" s="8">
-        <v>1.8897500000000001E-2</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1.9210600000000001E-2</v>
-      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -6775,21 +6663,10 @@
       <c r="E8">
         <v>15.6965</v>
       </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
-      <c r="I8" s="8">
-        <v>1.72582E-5</v>
-      </c>
-      <c r="J8" s="8">
-        <v>2.1095099999999999E-2</v>
-      </c>
-      <c r="K8" s="8">
-        <v>2.06854E-2</v>
-      </c>
-      <c r="L8" s="8">
-        <v>2.1003999999999998E-2</v>
-      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -6807,21 +6684,10 @@
       <c r="E9">
         <v>17.580100000000002</v>
       </c>
-      <c r="H9">
-        <v>17</v>
-      </c>
-      <c r="I9" s="8">
-        <v>1.9604200000000001E-5</v>
-      </c>
-      <c r="J9" s="8">
-        <v>2.2797899999999999E-2</v>
-      </c>
-      <c r="K9" s="8">
-        <v>2.2550199999999999E-2</v>
-      </c>
-      <c r="L9" s="8">
-        <v>2.2817199999999999E-2</v>
-      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -6839,21 +6705,10 @@
       <c r="E10">
         <v>28.2605</v>
       </c>
-      <c r="H10">
-        <v>18</v>
-      </c>
-      <c r="I10" s="8">
-        <v>2.10608E-5</v>
-      </c>
-      <c r="J10" s="8">
-        <v>2.4308900000000001E-2</v>
-      </c>
-      <c r="K10" s="8">
-        <v>2.4008000000000002E-2</v>
-      </c>
-      <c r="L10" s="8">
-        <v>2.4322799999999999E-2</v>
-      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -6871,21 +6726,10 @@
       <c r="E11">
         <v>21.329699999999999</v>
       </c>
-      <c r="H11">
-        <v>19</v>
-      </c>
-      <c r="I11" s="8">
-        <v>2.2053899999999999E-5</v>
-      </c>
-      <c r="J11" s="8">
-        <v>2.5604499999999999E-2</v>
-      </c>
-      <c r="K11" s="8">
-        <v>2.5282499999999999E-2</v>
-      </c>
-      <c r="L11" s="8">
-        <v>2.5841900000000001E-2</v>
-      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -6903,21 +6747,10 @@
       <c r="E12">
         <v>28.3064</v>
       </c>
-      <c r="H12">
-        <v>20</v>
-      </c>
-      <c r="I12" s="8">
-        <v>2.37478E-5</v>
-      </c>
-      <c r="J12" s="8">
-        <v>2.6956500000000001E-2</v>
-      </c>
-      <c r="K12" s="8">
-        <v>2.6532799999999999E-2</v>
-      </c>
-      <c r="L12" s="8">
-        <v>2.69736E-2</v>
-      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -6935,21 +6768,10 @@
       <c r="E13">
         <v>27.677499999999998</v>
       </c>
-      <c r="H13">
-        <v>21</v>
-      </c>
-      <c r="I13" s="8">
-        <v>2.4527200000000001E-5</v>
-      </c>
-      <c r="J13" s="8">
-        <v>2.8026499999999999E-2</v>
-      </c>
-      <c r="K13" s="8">
-        <v>2.7739300000000001E-2</v>
-      </c>
-      <c r="L13" s="8">
-        <v>2.8229299999999999E-2</v>
-      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -6967,21 +6789,10 @@
       <c r="E14">
         <v>28.334700000000002</v>
       </c>
-      <c r="H14">
-        <v>22</v>
-      </c>
-      <c r="I14" s="8">
-        <v>2.45715E-5</v>
-      </c>
-      <c r="J14" s="8">
-        <v>2.9020000000000001E-2</v>
-      </c>
-      <c r="K14" s="8">
-        <v>2.86988E-2</v>
-      </c>
-      <c r="L14" s="8">
-        <v>2.9266400000000001E-2</v>
-      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -6999,21 +6810,10 @@
       <c r="E15">
         <v>27.279499999999999</v>
       </c>
-      <c r="H15">
-        <v>23</v>
-      </c>
-      <c r="I15" s="8">
-        <v>2.5493499999999999E-5</v>
-      </c>
-      <c r="J15" s="8">
-        <v>3.0020600000000001E-2</v>
-      </c>
-      <c r="K15" s="8">
-        <v>2.9700299999999999E-2</v>
-      </c>
-      <c r="L15" s="8">
-        <v>3.00478E-2</v>
-      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -7031,21 +6831,10 @@
       <c r="E16">
         <v>26.128399999999999</v>
       </c>
-      <c r="H16">
-        <v>24</v>
-      </c>
-      <c r="I16" s="8">
-        <v>2.63375E-5</v>
-      </c>
-      <c r="J16" s="8">
-        <v>3.0884000000000002E-2</v>
-      </c>
-      <c r="K16" s="8">
-        <v>3.04934E-2</v>
-      </c>
-      <c r="L16" s="8">
-        <v>3.0930800000000001E-2</v>
-      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -7063,21 +6852,10 @@
       <c r="E17">
         <v>18.2364</v>
       </c>
-      <c r="H17">
-        <v>25</v>
-      </c>
-      <c r="I17" s="8">
-        <v>3.0784000000000002E-5</v>
-      </c>
-      <c r="J17" s="8">
-        <v>3.2534300000000002E-2</v>
-      </c>
-      <c r="K17" s="8">
-        <v>3.20176E-2</v>
-      </c>
-      <c r="L17" s="8">
-        <v>3.25417E-2</v>
-      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7087,10 +6865,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7104,9 +6882,9 @@
     <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -7117,20 +6895,8 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -7143,20 +6909,8 @@
       <c r="D2">
         <v>35.147399999999998</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>1.02335E-2</v>
-      </c>
-      <c r="I2">
-        <v>1.02626E-2</v>
-      </c>
-      <c r="J2">
-        <v>1.01584E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -7169,20 +6923,8 @@
       <c r="D3">
         <v>37.833599999999997</v>
       </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>1.11319E-2</v>
-      </c>
-      <c r="I3">
-        <v>1.10668E-2</v>
-      </c>
-      <c r="J3">
-        <v>1.10817E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -7195,20 +6937,8 @@
       <c r="D4">
         <v>39.604300000000002</v>
       </c>
-      <c r="G4">
-        <v>12</v>
-      </c>
-      <c r="H4">
-        <v>1.1772700000000001E-2</v>
-      </c>
-      <c r="I4">
-        <v>1.1776099999999999E-2</v>
-      </c>
-      <c r="J4">
-        <v>1.17436E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
@@ -7221,20 +6951,8 @@
       <c r="D5">
         <v>41.4116</v>
       </c>
-      <c r="G5">
-        <v>13</v>
-      </c>
-      <c r="H5">
-        <v>1.4319200000000001E-2</v>
-      </c>
-      <c r="I5">
-        <v>1.4334899999999999E-2</v>
-      </c>
-      <c r="J5">
-        <v>1.43351E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -7247,20 +6965,8 @@
       <c r="D6">
         <v>42.381300000000003</v>
       </c>
-      <c r="G6">
-        <v>14</v>
-      </c>
-      <c r="H6">
-        <v>1.6894699999999999E-2</v>
-      </c>
-      <c r="I6">
-        <v>1.6921499999999999E-2</v>
-      </c>
-      <c r="J6">
-        <v>1.69576E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -7273,20 +6979,8 @@
       <c r="D7">
         <v>44.272399999999998</v>
       </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7">
-        <v>1.9117800000000001E-2</v>
-      </c>
-      <c r="I7">
-        <v>1.9136899999999998E-2</v>
-      </c>
-      <c r="J7">
-        <v>1.91466E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16</v>
       </c>
@@ -7299,20 +6993,8 @@
       <c r="D8">
         <v>45.706699999999998</v>
       </c>
-      <c r="G8">
-        <v>16</v>
-      </c>
-      <c r="H8">
-        <v>2.1297E-2</v>
-      </c>
-      <c r="I8">
-        <v>2.1021700000000001E-2</v>
-      </c>
-      <c r="J8">
-        <v>2.1118000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>17</v>
       </c>
@@ -7325,20 +7007,8 @@
       <c r="D9">
         <v>46.763599999999997</v>
       </c>
-      <c r="G9">
-        <v>17</v>
-      </c>
-      <c r="H9">
-        <v>2.2907899999999998E-2</v>
-      </c>
-      <c r="I9">
-        <v>2.27598E-2</v>
-      </c>
-      <c r="J9">
-        <v>2.2889E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>18</v>
       </c>
@@ -7351,20 +7021,8 @@
       <c r="D10">
         <v>48.023699999999998</v>
       </c>
-      <c r="G10">
-        <v>18</v>
-      </c>
-      <c r="H10">
-        <v>2.4353E-2</v>
-      </c>
-      <c r="I10">
-        <v>2.4426099999999999E-2</v>
-      </c>
-      <c r="J10">
-        <v>2.4430500000000001E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>19</v>
       </c>
@@ -7377,20 +7035,8 @@
       <c r="D11">
         <v>49.159100000000002</v>
       </c>
-      <c r="G11">
-        <v>19</v>
-      </c>
-      <c r="H11">
-        <v>2.5747800000000001E-2</v>
-      </c>
-      <c r="I11">
-        <v>2.5762199999999999E-2</v>
-      </c>
-      <c r="J11">
-        <v>2.5927800000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20</v>
       </c>
@@ -7403,20 +7049,8 @@
       <c r="D12">
         <v>50.256300000000003</v>
       </c>
-      <c r="G12">
-        <v>20</v>
-      </c>
-      <c r="H12">
-        <v>2.7094099999999999E-2</v>
-      </c>
-      <c r="I12">
-        <v>2.7157799999999999E-2</v>
-      </c>
-      <c r="J12">
-        <v>2.7055800000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>21</v>
       </c>
@@ -7429,20 +7063,8 @@
       <c r="D13">
         <v>50.856499999999997</v>
       </c>
-      <c r="G13">
-        <v>21</v>
-      </c>
-      <c r="H13">
-        <v>2.8301400000000001E-2</v>
-      </c>
-      <c r="I13">
-        <v>2.8126200000000001E-2</v>
-      </c>
-      <c r="J13">
-        <v>2.8239799999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22</v>
       </c>
@@ -7455,20 +7077,8 @@
       <c r="D14">
         <v>52.049100000000003</v>
       </c>
-      <c r="G14">
-        <v>22</v>
-      </c>
-      <c r="H14">
-        <v>2.9277600000000001E-2</v>
-      </c>
-      <c r="I14">
-        <v>2.9260399999999999E-2</v>
-      </c>
-      <c r="J14">
-        <v>2.9259500000000001E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>23</v>
       </c>
@@ -7481,20 +7091,8 @@
       <c r="D15">
         <v>52.718200000000003</v>
       </c>
-      <c r="G15">
-        <v>23</v>
-      </c>
-      <c r="H15">
-        <v>3.0289799999999999E-2</v>
-      </c>
-      <c r="I15">
-        <v>3.0218700000000001E-2</v>
-      </c>
-      <c r="J15">
-        <v>3.01909E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>24</v>
       </c>
@@ -7507,20 +7105,8 @@
       <c r="D16">
         <v>53.509399999999999</v>
       </c>
-      <c r="G16">
-        <v>24</v>
-      </c>
-      <c r="H16">
-        <v>3.1122799999999999E-2</v>
-      </c>
-      <c r="I16">
-        <v>3.10554E-2</v>
-      </c>
-      <c r="J16">
-        <v>3.0977899999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>25</v>
       </c>
@@ -7532,18 +7118,6 @@
       </c>
       <c r="D17">
         <v>54.360199999999999</v>
-      </c>
-      <c r="G17">
-        <v>25</v>
-      </c>
-      <c r="H17">
-        <v>3.2617100000000003E-2</v>
-      </c>
-      <c r="I17">
-        <v>3.2721300000000002E-2</v>
-      </c>
-      <c r="J17">
-        <v>3.2541199999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7554,10 +7128,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7571,9 +7145,9 @@
     <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -7587,23 +7161,8 @@
       <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -7619,23 +7178,8 @@
       <c r="E2">
         <v>31.537500000000001</v>
       </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>0.81020300000000001</v>
-      </c>
-      <c r="J2">
-        <v>1.2933099999999999E-2</v>
-      </c>
-      <c r="K2">
-        <v>1.29309E-2</v>
-      </c>
-      <c r="L2">
-        <v>1.2933E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -7651,23 +7195,8 @@
       <c r="E3">
         <v>28.970700000000001</v>
       </c>
-      <c r="H3">
-        <v>11</v>
-      </c>
-      <c r="I3">
-        <v>0.80975699999999995</v>
-      </c>
-      <c r="J3">
-        <v>1.5352299999999999E-2</v>
-      </c>
-      <c r="K3">
-        <v>1.53508E-2</v>
-      </c>
-      <c r="L3">
-        <v>1.5352599999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -7683,23 +7212,8 @@
       <c r="E4">
         <v>28.620100000000001</v>
       </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>0.809361</v>
-      </c>
-      <c r="J4">
-        <v>1.7320700000000001E-2</v>
-      </c>
-      <c r="K4">
-        <v>1.7318900000000002E-2</v>
-      </c>
-      <c r="L4">
-        <v>1.7320599999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
@@ -7715,23 +7229,8 @@
       <c r="E5">
         <v>19.258099999999999</v>
       </c>
-      <c r="H5">
-        <v>13</v>
-      </c>
-      <c r="I5">
-        <v>0.80906500000000003</v>
-      </c>
-      <c r="J5">
-        <v>1.9015500000000001E-2</v>
-      </c>
-      <c r="K5">
-        <v>1.90122E-2</v>
-      </c>
-      <c r="L5">
-        <v>1.90157E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -7747,23 +7246,8 @@
       <c r="E6">
         <v>16.030999999999999</v>
       </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>0.80875699999999995</v>
-      </c>
-      <c r="J6">
-        <v>2.04744E-2</v>
-      </c>
-      <c r="K6">
-        <v>2.04733E-2</v>
-      </c>
-      <c r="L6">
-        <v>2.0476399999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -7779,23 +7263,8 @@
       <c r="E7">
         <v>15.647600000000001</v>
       </c>
-      <c r="H7">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>0.80847599999999997</v>
-      </c>
-      <c r="J7">
-        <v>2.17673E-2</v>
-      </c>
-      <c r="K7">
-        <v>2.17637E-2</v>
-      </c>
-      <c r="L7">
-        <v>2.1767600000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16</v>
       </c>
@@ -7811,23 +7280,8 @@
       <c r="E8">
         <v>14.6526</v>
       </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
-      <c r="I8">
-        <v>0.80826399999999998</v>
-      </c>
-      <c r="J8">
-        <v>2.2870999999999999E-2</v>
-      </c>
-      <c r="K8">
-        <v>2.2868200000000002E-2</v>
-      </c>
-      <c r="L8">
-        <v>2.28714E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>17</v>
       </c>
@@ -7843,23 +7297,8 @@
       <c r="E9">
         <v>9.5356699999999996</v>
       </c>
-      <c r="H9">
-        <v>17</v>
-      </c>
-      <c r="I9">
-        <v>0.80745199999999995</v>
-      </c>
-      <c r="J9">
-        <v>2.7241999999999999E-2</v>
-      </c>
-      <c r="K9">
-        <v>2.7238100000000001E-2</v>
-      </c>
-      <c r="L9">
-        <v>2.7242499999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>18</v>
       </c>
@@ -7875,23 +7314,8 @@
       <c r="E10">
         <v>12.3348</v>
       </c>
-      <c r="H10">
-        <v>18</v>
-      </c>
-      <c r="I10">
-        <v>0.80638399999999999</v>
-      </c>
-      <c r="J10">
-        <v>3.3055099999999997E-2</v>
-      </c>
-      <c r="K10">
-        <v>3.3050700000000002E-2</v>
-      </c>
-      <c r="L10">
-        <v>3.3055000000000001E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>19</v>
       </c>
@@ -7907,23 +7331,8 @@
       <c r="E11">
         <v>11.848800000000001</v>
       </c>
-      <c r="H11">
-        <v>19</v>
-      </c>
-      <c r="I11">
-        <v>0.80538900000000002</v>
-      </c>
-      <c r="J11">
-        <v>3.8324400000000002E-2</v>
-      </c>
-      <c r="K11">
-        <v>3.8319600000000002E-2</v>
-      </c>
-      <c r="L11">
-        <v>3.8325699999999997E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20</v>
       </c>
@@ -7939,23 +7348,8 @@
       <c r="E12">
         <v>11.2196</v>
       </c>
-      <c r="H12">
-        <v>20</v>
-      </c>
-      <c r="I12">
-        <v>0.80449400000000004</v>
-      </c>
-      <c r="J12">
-        <v>4.31321E-2</v>
-      </c>
-      <c r="K12">
-        <v>4.3127199999999997E-2</v>
-      </c>
-      <c r="L12">
-        <v>4.3133600000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>21</v>
       </c>
@@ -7971,23 +7365,8 @@
       <c r="E13">
         <v>11.2858</v>
       </c>
-      <c r="H13">
-        <v>21</v>
-      </c>
-      <c r="I13">
-        <v>0.80369100000000004</v>
-      </c>
-      <c r="J13">
-        <v>4.7421900000000003E-2</v>
-      </c>
-      <c r="K13">
-        <v>4.7417399999999998E-2</v>
-      </c>
-      <c r="L13">
-        <v>4.7423399999999998E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22</v>
       </c>
@@ -8003,23 +7382,8 @@
       <c r="E14">
         <v>11.1633</v>
       </c>
-      <c r="H14">
-        <v>22</v>
-      </c>
-      <c r="I14">
-        <v>0.80292200000000002</v>
-      </c>
-      <c r="J14">
-        <v>5.1415700000000002E-2</v>
-      </c>
-      <c r="K14">
-        <v>5.1408299999999997E-2</v>
-      </c>
-      <c r="L14">
-        <v>5.1416099999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>23</v>
       </c>
@@ -8035,23 +7399,8 @@
       <c r="E15">
         <v>11.1981</v>
       </c>
-      <c r="H15">
-        <v>23</v>
-      </c>
-      <c r="I15">
-        <v>0.80221600000000004</v>
-      </c>
-      <c r="J15">
-        <v>5.5075600000000002E-2</v>
-      </c>
-      <c r="K15">
-        <v>5.5068499999999999E-2</v>
-      </c>
-      <c r="L15">
-        <v>5.5075600000000002E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>24</v>
       </c>
@@ -8067,23 +7416,8 @@
       <c r="E16">
         <v>10.7796</v>
       </c>
-      <c r="H16">
-        <v>24</v>
-      </c>
-      <c r="I16">
-        <v>0.80158499999999999</v>
-      </c>
-      <c r="J16">
-        <v>5.8482699999999999E-2</v>
-      </c>
-      <c r="K16">
-        <v>5.8473900000000002E-2</v>
-      </c>
-      <c r="L16">
-        <v>5.8482800000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>25</v>
       </c>
@@ -8098,21 +7432,6 @@
       </c>
       <c r="E17">
         <v>10.866899999999999</v>
-      </c>
-      <c r="H17">
-        <v>25</v>
-      </c>
-      <c r="I17">
-        <v>0.800979</v>
-      </c>
-      <c r="J17">
-        <v>6.1609200000000003E-2</v>
-      </c>
-      <c r="K17">
-        <v>6.1601700000000002E-2</v>
-      </c>
-      <c r="L17">
-        <v>6.1610400000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8123,10 +7442,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8140,9 +7459,9 @@
     <col min="14" max="14" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -8151,34 +7470,16 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -8197,26 +7498,8 @@
       <c r="F2">
         <v>90.348299999999995</v>
       </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>1.2933E-2</v>
-      </c>
-      <c r="K2">
-        <v>1.2933E-2</v>
-      </c>
-      <c r="L2">
-        <v>1.2933E-2</v>
-      </c>
-      <c r="M2">
-        <v>1.2933E-2</v>
-      </c>
-      <c r="N2">
-        <v>1.2933099999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11</v>
       </c>
@@ -8235,26 +7518,8 @@
       <c r="F3">
         <v>90.518600000000006</v>
       </c>
-      <c r="I3">
-        <v>11</v>
-      </c>
-      <c r="J3">
-        <v>1.5352599999999999E-2</v>
-      </c>
-      <c r="K3">
-        <v>1.53525E-2</v>
-      </c>
-      <c r="L3">
-        <v>1.5352599999999999E-2</v>
-      </c>
-      <c r="M3">
-        <v>1.5352599999999999E-2</v>
-      </c>
-      <c r="N3">
-        <v>1.53525E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -8273,26 +7538,8 @@
       <c r="F4">
         <v>93.240600000000001</v>
       </c>
-      <c r="I4">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>1.7320599999999998E-2</v>
-      </c>
-      <c r="K4">
-        <v>1.7320599999999998E-2</v>
-      </c>
-      <c r="L4">
-        <v>1.7320599999999998E-2</v>
-      </c>
-      <c r="M4">
-        <v>1.7320599999999998E-2</v>
-      </c>
-      <c r="N4">
-        <v>1.7320599999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>13</v>
       </c>
@@ -8311,26 +7558,8 @@
       <c r="F5">
         <v>93.988</v>
       </c>
-      <c r="I5">
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <v>1.90157E-2</v>
-      </c>
-      <c r="K5">
-        <v>1.90157E-2</v>
-      </c>
-      <c r="L5">
-        <v>1.90157E-2</v>
-      </c>
-      <c r="M5">
-        <v>1.90157E-2</v>
-      </c>
-      <c r="N5">
-        <v>1.90157E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -8349,26 +7578,8 @@
       <c r="F6">
         <v>101.405</v>
       </c>
-      <c r="I6">
-        <v>14</v>
-      </c>
-      <c r="J6">
-        <v>2.0476500000000002E-2</v>
-      </c>
-      <c r="K6">
-        <v>2.04767E-2</v>
-      </c>
-      <c r="L6">
-        <v>2.0476500000000002E-2</v>
-      </c>
-      <c r="M6">
-        <v>2.0476500000000002E-2</v>
-      </c>
-      <c r="N6">
-        <v>2.0476500000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -8387,26 +7598,8 @@
       <c r="F7">
         <v>97.145200000000003</v>
       </c>
-      <c r="I7">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>2.1767499999999999E-2</v>
-      </c>
-      <c r="K7">
-        <v>2.1767600000000002E-2</v>
-      </c>
-      <c r="L7">
-        <v>2.1767600000000002E-2</v>
-      </c>
-      <c r="M7">
-        <v>2.1767600000000002E-2</v>
-      </c>
-      <c r="N7">
-        <v>2.1767499999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16</v>
       </c>
@@ -8425,26 +7618,8 @@
       <c r="F8">
         <v>103.498</v>
       </c>
-      <c r="I8">
-        <v>16</v>
-      </c>
-      <c r="J8">
-        <v>2.2871499999999999E-2</v>
-      </c>
-      <c r="K8">
-        <v>2.28714E-2</v>
-      </c>
-      <c r="L8">
-        <v>2.28714E-2</v>
-      </c>
-      <c r="M8">
-        <v>2.28714E-2</v>
-      </c>
-      <c r="N8">
-        <v>2.2871499999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>17</v>
       </c>
@@ -8463,26 +7638,8 @@
       <c r="F9">
         <v>97.877799999999993</v>
       </c>
-      <c r="I9">
-        <v>17</v>
-      </c>
-      <c r="J9">
-        <v>2.7244299999999999E-2</v>
-      </c>
-      <c r="K9">
-        <v>2.7242599999999999E-2</v>
-      </c>
-      <c r="L9">
-        <v>2.7242599999999999E-2</v>
-      </c>
-      <c r="M9">
-        <v>2.7242599999999999E-2</v>
-      </c>
-      <c r="N9">
-        <v>2.7242599999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>18</v>
       </c>
@@ -8501,26 +7658,8 @@
       <c r="F10">
         <v>107.827</v>
       </c>
-      <c r="I10">
-        <v>18</v>
-      </c>
-      <c r="J10">
-        <v>3.3056700000000001E-2</v>
-      </c>
-      <c r="K10">
-        <v>3.3056799999999997E-2</v>
-      </c>
-      <c r="L10">
-        <v>3.3056799999999997E-2</v>
-      </c>
-      <c r="M10">
-        <v>3.3056799999999997E-2</v>
-      </c>
-      <c r="N10">
-        <v>3.3056799999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>19</v>
       </c>
@@ -8539,26 +7678,8 @@
       <c r="F11">
         <v>110.166</v>
       </c>
-      <c r="I11">
-        <v>19</v>
-      </c>
-      <c r="J11">
-        <v>3.83258E-2</v>
-      </c>
-      <c r="K11">
-        <v>3.8325699999999997E-2</v>
-      </c>
-      <c r="L11">
-        <v>3.83258E-2</v>
-      </c>
-      <c r="M11">
-        <v>3.83258E-2</v>
-      </c>
-      <c r="N11">
-        <v>3.8325699999999997E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20</v>
       </c>
@@ -8577,26 +7698,8 @@
       <c r="F12">
         <v>101.389</v>
       </c>
-      <c r="I12">
-        <v>20</v>
-      </c>
-      <c r="J12">
-        <v>4.3133699999999997E-2</v>
-      </c>
-      <c r="K12">
-        <v>4.3133699999999997E-2</v>
-      </c>
-      <c r="L12">
-        <v>4.3133699999999997E-2</v>
-      </c>
-      <c r="M12">
-        <v>4.3133699999999997E-2</v>
-      </c>
-      <c r="N12">
-        <v>4.3133699999999997E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>21</v>
       </c>
@@ -8615,26 +7718,8 @@
       <c r="F13">
         <v>110.58799999999999</v>
       </c>
-      <c r="I13">
-        <v>21</v>
-      </c>
-      <c r="J13">
-        <v>4.7423899999999998E-2</v>
-      </c>
-      <c r="K13">
-        <v>4.7423899999999998E-2</v>
-      </c>
-      <c r="L13">
-        <v>4.7424000000000001E-2</v>
-      </c>
-      <c r="M13">
-        <v>4.7424000000000001E-2</v>
-      </c>
-      <c r="N13">
-        <v>4.7424000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22</v>
       </c>
@@ -8653,26 +7738,8 @@
       <c r="F14">
         <v>107.85599999999999</v>
       </c>
-      <c r="I14">
-        <v>22</v>
-      </c>
-      <c r="J14">
-        <v>5.1417299999999999E-2</v>
-      </c>
-      <c r="K14">
-        <v>5.1417299999999999E-2</v>
-      </c>
-      <c r="L14">
-        <v>5.1417299999999999E-2</v>
-      </c>
-      <c r="M14">
-        <v>5.1417299999999999E-2</v>
-      </c>
-      <c r="N14">
-        <v>5.1417299999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>23</v>
       </c>
@@ -8691,26 +7758,8 @@
       <c r="F15">
         <v>100.39100000000001</v>
       </c>
-      <c r="I15">
-        <v>23</v>
-      </c>
-      <c r="J15">
-        <v>5.5076100000000003E-2</v>
-      </c>
-      <c r="K15">
-        <v>5.5076100000000003E-2</v>
-      </c>
-      <c r="L15">
-        <v>5.5076100000000003E-2</v>
-      </c>
-      <c r="M15">
-        <v>5.5076100000000003E-2</v>
-      </c>
-      <c r="N15">
-        <v>5.5076100000000003E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>24</v>
       </c>
@@ -8729,26 +7778,8 @@
       <c r="F16">
         <v>101.22499999999999</v>
       </c>
-      <c r="I16">
-        <v>24</v>
-      </c>
-      <c r="J16">
-        <v>5.8483199999999999E-2</v>
-      </c>
-      <c r="K16">
-        <v>5.8483300000000002E-2</v>
-      </c>
-      <c r="L16">
-        <v>5.8483100000000003E-2</v>
-      </c>
-      <c r="M16">
-        <v>5.8483100000000003E-2</v>
-      </c>
-      <c r="N16">
-        <v>5.8483100000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>25</v>
       </c>
@@ -8766,24 +7797,6 @@
       </c>
       <c r="F17">
         <v>101.008</v>
-      </c>
-      <c r="I17">
-        <v>25</v>
-      </c>
-      <c r="J17">
-        <v>6.1610600000000001E-2</v>
-      </c>
-      <c r="K17">
-        <v>6.1610699999999997E-2</v>
-      </c>
-      <c r="L17">
-        <v>6.1610600000000001E-2</v>
-      </c>
-      <c r="M17">
-        <v>6.1610600000000001E-2</v>
-      </c>
-      <c r="N17">
-        <v>6.1610600000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8797,7 +7810,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8812,19 +7825,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -9123,28 +8136,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
       </c>
       <c r="I1" t="s">
         <v>23</v>
@@ -9675,7 +8688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -9689,19 +8702,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>